<commit_message>
Getting started on analysing field trial data
</commit_message>
<xml_diff>
--- a/Data/GEF Field Trial/AllometricModels.xlsx
+++ b/Data/GEF Field Trial/AllometricModels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Allometric Models" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="110">
   <si>
     <t>Aloe</t>
   </si>
@@ -1009,7 +1009,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="A5A5A5"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1266,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1281,7 +1281,9 @@
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="C1" s="2" t="s">
         <v>76</v>
       </c>
@@ -3109,7 +3111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
busy trying to get new NGI image orthorect to work
</commit_message>
<xml_diff>
--- a/Data/GEF Field Trial/AllometricModels.xlsx
+++ b/Data/GEF Field Trial/AllometricModels.xlsx
@@ -1267,7 +1267,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3116,6 +3116,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">

</xml_diff>

<commit_message>
bugfixes and wet dry ratios added
</commit_message>
<xml_diff>
--- a/Data/GEF Field Trial/AllometricModels.xlsx
+++ b/Data/GEF Field Trial/AllometricModels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Allometric Models" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="106">
   <si>
     <t>Aloe</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Galenia</t>
   </si>
   <si>
-    <t>fliformis</t>
-  </si>
-  <si>
     <t>Grewia</t>
   </si>
   <si>
@@ -236,9 +233,6 @@
   </si>
   <si>
     <t>Ruschia</t>
-  </si>
-  <si>
-    <t>multflora</t>
   </si>
   <si>
     <t>Schotia</t>
@@ -342,9 +336,6 @@
     <t>SE</t>
   </si>
   <si>
-    <t>mesembryanthoides</t>
-  </si>
-  <si>
     <t>filiformis</t>
   </si>
   <si>
@@ -364,9 +355,6 @@
   </si>
   <si>
     <t>longispina</t>
-  </si>
-  <si>
-    <t>karroo</t>
   </si>
   <si>
     <t>Putterlickia</t>
@@ -922,6 +910,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -941,7 +997,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="A5A5A5"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1198,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1211,49 +1267,49 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="O1" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1476,7 +1532,7 @@
         <v>1.01</v>
       </c>
       <c r="O6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1792,7 +1848,7 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
@@ -1831,7 +1887,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="O14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -2147,7 +2203,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -2188,10 +2244,10 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
         <v>44</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -2232,10 +2288,10 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
         <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>47</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -2276,7 +2332,7 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -2320,10 +2376,10 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
         <v>49</v>
-      </c>
-      <c r="B26" t="s">
-        <v>50</v>
       </c>
       <c r="C26" t="s">
         <v>32</v>
@@ -2364,13 +2420,13 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
@@ -2406,15 +2462,15 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="O27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
         <v>52</v>
-      </c>
-      <c r="B28" t="s">
-        <v>53</v>
       </c>
       <c r="C28" t="s">
         <v>32</v>
@@ -2455,13 +2511,13 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
         <v>54</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>55</v>
-      </c>
-      <c r="C29" t="s">
-        <v>56</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -2499,10 +2555,10 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -2541,12 +2597,12 @@
         <v>1.03</v>
       </c>
       <c r="O30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -2590,10 +2646,10 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
         <v>28</v>
@@ -2632,15 +2688,15 @@
         <v>1.05</v>
       </c>
       <c r="O32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
         <v>60</v>
-      </c>
-      <c r="B33" t="s">
-        <v>61</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -2681,10 +2737,10 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
         <v>62</v>
-      </c>
-      <c r="B34" t="s">
-        <v>63</v>
       </c>
       <c r="C34" t="s">
         <v>32</v>
@@ -2725,10 +2781,10 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" t="s">
         <v>64</v>
-      </c>
-      <c r="B35" t="s">
-        <v>65</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -2769,10 +2825,10 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" t="s">
         <v>66</v>
-      </c>
-      <c r="B36" t="s">
-        <v>67</v>
       </c>
       <c r="C36" t="s">
         <v>32</v>
@@ -2813,10 +2869,10 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
@@ -2857,13 +2913,13 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" t="s">
         <v>69</v>
       </c>
-      <c r="B38" t="s">
-        <v>70</v>
-      </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
@@ -2901,10 +2957,10 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C39" t="s">
         <v>32</v>
@@ -2945,10 +3001,10 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
@@ -2989,10 +3045,10 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
         <v>28</v>
@@ -3031,7 +3087,7 @@
         <v>1.02</v>
       </c>
       <c r="O41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3043,34 +3099,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3178,7 +3234,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3218,7 +3274,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
@@ -3338,7 +3394,7 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
         <v>32</v>
@@ -3355,10 +3411,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -3375,10 +3431,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -3395,10 +3451,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
         <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -3415,7 +3471,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -3435,10 +3491,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -3455,10 +3511,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
         <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>32</v>
@@ -3475,13 +3531,13 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
         <v>54</v>
       </c>
-      <c r="B22" t="s">
-        <v>55</v>
-      </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D22">
         <v>6</v>
@@ -3495,10 +3551,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
         <v>32</v>
@@ -3515,7 +3571,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -3535,10 +3591,10 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -3555,10 +3611,10 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" t="s">
-        <v>61</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
@@ -3575,10 +3631,10 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
         <v>66</v>
-      </c>
-      <c r="B27" t="s">
-        <v>67</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -3595,10 +3651,10 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
         <v>32</v>
@@ -3615,10 +3671,10 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -3635,10 +3691,10 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
@@ -3655,10 +3711,10 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
added trial to consolidated sheet added mp's searsia model (r2=0.5 so suspect)
</commit_message>
<xml_diff>
--- a/Data/GEF Field Trial/AllometricModels.xlsx
+++ b/Data/GEF Field Trial/AllometricModels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Allometric Models" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="109">
   <si>
     <t>Aloe</t>
   </si>
@@ -359,12 +359,21 @@
   <si>
     <t>Putterlickia</t>
   </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log10 y (C (kg) = 1.1012(Log10 canopy area (m2)) - 0.2938 </t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,6 +525,12 @@
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="CMSY7"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -859,10 +874,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -997,7 +1013,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="A5A5A5"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1252,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2691,7 +2707,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -2735,7 +2751,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2779,7 +2795,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -2823,7 +2839,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2867,7 +2883,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>105</v>
       </c>
@@ -2911,7 +2927,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -2955,7 +2971,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -2999,7 +3015,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -3043,7 +3059,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -3090,8 +3106,41 @@
         <v>86</v>
       </c>
     </row>
+    <row r="42" spans="1:16">
+      <c r="A42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42">
+        <v>24</v>
+      </c>
+      <c r="F42">
+        <v>0.50770000000000004</v>
+      </c>
+      <c r="G42">
+        <v>1.1012</v>
+      </c>
+      <c r="H42">
+        <v>-0.29380000000000001</v>
+      </c>
+      <c r="O42" t="s">
+        <v>86</v>
+      </c>
+      <c r="P42" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3099,8 +3148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>